<commit_message>
completed job,user for admin ui
</commit_message>
<xml_diff>
--- a/src/assets/template/job.xlsx
+++ b/src/assets/template/job.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\IT\springrest\03-react-vite-jobhunter\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51769350-F0BD-4A60-88CB-47B5D55474CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470EEA3C-1B30-431D-9245-6C8FAC7EEE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{825C882F-18F0-4041-B822-7E59F53330AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{825C882F-18F0-4041-B822-7E59F53330AE}"/>
   </bookViews>
   <sheets>
     <sheet name="export-jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -101,13 +101,46 @@
   </si>
   <si>
     <t>Dev Java123</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>374 pham van dong</t>
+  </si>
+  <si>
+    <t>375 pham van dong</t>
+  </si>
+  <si>
+    <t>376 pham van dong</t>
+  </si>
+  <si>
+    <t>377 pham van dong</t>
+  </si>
+  <si>
+    <t>378 pham van dong</t>
+  </si>
+  <si>
+    <t>379 pham van dong</t>
+  </si>
+  <si>
+    <t>380 pham van dong</t>
+  </si>
+  <si>
+    <t>381 pham van dong</t>
+  </si>
+  <si>
+    <t>382 pham van dong</t>
+  </si>
+  <si>
+    <t>383 pham van dong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +271,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -961,15 +1000,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B2B66F-8DF3-43D7-B40A-183136C8B40B}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -977,384 +1016,418 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
         <v>10000000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
         <v>123123123</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>123123</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
         <v>10000000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
         <v>10000000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
         <v>10000000</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
         <v>12312312</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1231</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
         <v>10000000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
       <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
         <v>10000000</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10">
         <v>10000000</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
         <v>10000000</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>